<commit_message>
DDL, DML e DQL(1.2, 1.3, 1.4)
</commit_message>
<xml_diff>
--- a/exercicios/1.3-exercicio-pclinics/04_modelagem_fisico.xlsx
+++ b/exercicios/1.3-exercicio-pclinics/04_modelagem_fisico.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\HD\SENAI-2ºT\sprint-1\exercicios\1.3-exercicio-pclinics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FCFFFDF-27C9-450B-9089-7E0FF4FE1CD0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{310B1233-4A64-430A-B332-38EA8117EF24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1470" yWindow="1470" windowWidth="15300" windowHeight="7995" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
@@ -287,9 +287,6 @@
   </cellStyleXfs>
   <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -298,9 +295,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -308,9 +302,6 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -321,9 +312,6 @@
     <xf numFmtId="16" fontId="0" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -332,9 +320,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -343,14 +328,8 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="18" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="20" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="21" borderId="0" xfId="0" applyFill="1"/>
@@ -361,6 +340,27 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="22" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -652,7 +652,7 @@
   <dimension ref="A1:N9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O10" sqref="O10"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -666,232 +666,232 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="D1" s="6" t="s">
+      <c r="B1" s="28"/>
+      <c r="D1" s="29" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
-      <c r="H1" s="10" t="s">
+      <c r="E1" s="29"/>
+      <c r="F1" s="29"/>
+      <c r="H1" s="30" t="s">
         <v>10</v>
       </c>
-      <c r="I1" s="10"/>
-      <c r="J1" s="10"/>
-      <c r="K1" s="10"/>
-      <c r="M1" s="28" t="s">
+      <c r="I1" s="30"/>
+      <c r="J1" s="30"/>
+      <c r="K1" s="30"/>
+      <c r="M1" s="27" t="s">
         <v>28</v>
       </c>
-      <c r="N1" s="28"/>
+      <c r="N1" s="27"/>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" s="7" t="s">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="F2" s="7" t="s">
+      <c r="E2" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="F2" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="H2" s="11" t="s">
+      <c r="H2" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="I2" s="12" t="s">
+      <c r="I2" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="J2" s="11" t="s">
+      <c r="J2" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="K2" s="11" t="s">
+      <c r="K2" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="M2" s="29" t="s">
+      <c r="M2" s="22" t="s">
         <v>18</v>
       </c>
-      <c r="N2" s="30" t="s">
+      <c r="N2" s="23" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A3" s="4">
-        <v>1</v>
-      </c>
-      <c r="B3" s="5" t="s">
+      <c r="A3" s="3">
+        <v>1</v>
+      </c>
+      <c r="B3" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="9">
-        <v>1</v>
-      </c>
-      <c r="E3" s="9">
-        <v>2</v>
-      </c>
-      <c r="F3" s="9" t="s">
+      <c r="D3" s="7">
+        <v>1</v>
+      </c>
+      <c r="E3" s="7">
+        <v>2</v>
+      </c>
+      <c r="F3" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="H3" s="13">
-        <v>1</v>
-      </c>
-      <c r="I3" s="13">
-        <v>2</v>
-      </c>
-      <c r="J3" s="13">
-        <v>1</v>
-      </c>
-      <c r="K3" s="14">
+      <c r="H3" s="10">
+        <v>1</v>
+      </c>
+      <c r="I3" s="10">
+        <v>2</v>
+      </c>
+      <c r="J3" s="10">
+        <v>1</v>
+      </c>
+      <c r="K3" s="11">
         <v>44412</v>
       </c>
-      <c r="M3" s="31">
-        <v>1</v>
-      </c>
-      <c r="N3" s="32" t="s">
+      <c r="M3" s="24">
+        <v>1</v>
+      </c>
+      <c r="N3" s="25" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A4" s="4">
-        <v>2</v>
-      </c>
-      <c r="B4" s="5" t="s">
+      <c r="A4" s="3">
+        <v>2</v>
+      </c>
+      <c r="B4" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="9">
-        <v>2</v>
-      </c>
-      <c r="E4" s="9">
-        <v>1</v>
-      </c>
-      <c r="F4" s="9" t="s">
+      <c r="D4" s="7">
+        <v>2</v>
+      </c>
+      <c r="E4" s="7">
+        <v>1</v>
+      </c>
+      <c r="F4" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="H4" s="13">
-        <v>2</v>
-      </c>
-      <c r="I4" s="13">
-        <v>1</v>
-      </c>
-      <c r="J4" s="13">
-        <v>2</v>
-      </c>
-      <c r="K4" s="14">
+      <c r="H4" s="10">
+        <v>2</v>
+      </c>
+      <c r="I4" s="10">
+        <v>1</v>
+      </c>
+      <c r="J4" s="10">
+        <v>2</v>
+      </c>
+      <c r="K4" s="11">
         <v>44411</v>
       </c>
-      <c r="M4" s="31">
-        <v>2</v>
-      </c>
-      <c r="N4" s="32" t="s">
+      <c r="M4" s="24">
+        <v>2</v>
+      </c>
+      <c r="N4" s="25" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A6" s="15" t="s">
+      <c r="A6" s="31" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="15"/>
-      <c r="C6" s="15"/>
-      <c r="E6" s="20" t="s">
+      <c r="B6" s="31"/>
+      <c r="C6" s="31"/>
+      <c r="E6" s="32" t="s">
         <v>19</v>
       </c>
-      <c r="F6" s="20"/>
-      <c r="H6" s="25" t="s">
+      <c r="F6" s="32"/>
+      <c r="H6" s="26" t="s">
         <v>27</v>
       </c>
-      <c r="I6" s="25"/>
-      <c r="J6" s="25"/>
-      <c r="K6" s="25"/>
+      <c r="I6" s="26"/>
+      <c r="J6" s="26"/>
+      <c r="K6" s="26"/>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A7" s="16" t="s">
+      <c r="A7" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="B7" s="17" t="s">
+      <c r="B7" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="C7" s="16" t="s">
+      <c r="C7" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="E7" s="21" t="s">
+      <c r="E7" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="F7" s="22" t="s">
+      <c r="F7" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="H7" s="26" t="s">
+      <c r="H7" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="I7" s="26" t="s">
+      <c r="I7" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="J7" s="26" t="s">
+      <c r="J7" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="K7" s="26" t="s">
+      <c r="K7" s="20" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A8" s="18">
-        <v>1</v>
-      </c>
-      <c r="B8" s="19" t="s">
+      <c r="A8" s="14">
+        <v>1</v>
+      </c>
+      <c r="B8" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="C8" s="18">
-        <v>1</v>
-      </c>
-      <c r="E8" s="23">
-        <v>1</v>
-      </c>
-      <c r="F8" s="24" t="s">
+      <c r="C8" s="14">
+        <v>1</v>
+      </c>
+      <c r="E8" s="18">
+        <v>1</v>
+      </c>
+      <c r="F8" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="H8" s="27">
-        <v>1</v>
-      </c>
-      <c r="I8" s="27">
-        <v>2</v>
-      </c>
-      <c r="J8" s="27">
-        <v>1</v>
-      </c>
-      <c r="K8" s="27" t="s">
+      <c r="H8" s="21">
+        <v>1</v>
+      </c>
+      <c r="I8" s="21">
+        <v>2</v>
+      </c>
+      <c r="J8" s="21">
+        <v>1</v>
+      </c>
+      <c r="K8" s="21" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A9" s="18">
-        <v>2</v>
-      </c>
-      <c r="B9" s="19" t="s">
+      <c r="A9" s="14">
+        <v>2</v>
+      </c>
+      <c r="B9" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="C9" s="18">
-        <v>2</v>
-      </c>
-      <c r="E9" s="23">
-        <v>2</v>
-      </c>
-      <c r="F9" s="24" t="s">
+      <c r="C9" s="14">
+        <v>2</v>
+      </c>
+      <c r="E9" s="18">
+        <v>2</v>
+      </c>
+      <c r="F9" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="H9" s="27">
-        <v>2</v>
-      </c>
-      <c r="I9" s="27">
-        <v>1</v>
-      </c>
-      <c r="J9" s="27">
-        <v>2</v>
-      </c>
-      <c r="K9" s="27" t="s">
+      <c r="H9" s="21">
+        <v>2</v>
+      </c>
+      <c r="I9" s="21">
+        <v>1</v>
+      </c>
+      <c r="J9" s="21">
+        <v>2</v>
+      </c>
+      <c r="K9" s="21" t="s">
         <v>26</v>
       </c>
     </row>

</xml_diff>